<commit_message>
tweet zamani ve v2 ayarlandi
</commit_message>
<xml_diff>
--- a/YLSYDer_programlari/ProgramControl.xlsx
+++ b/YLSYDer_programlari/ProgramControl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanercokyasar/Desktop/TBB/YLSYDer_programlari copy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanercokyasar/YLSYder/YLSYDer_programlari/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A433191-B67D-7545-98FA-8BE6CE98FC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA9CD0C-674B-7547-9C96-A596DEC3DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>api_key</t>
   </si>
@@ -34,20 +34,56 @@
     <t>access_token_secret</t>
   </si>
   <si>
+    <t>keyword1</t>
+  </si>
+  <si>
+    <t>sabitkur</t>
+  </si>
+  <si>
+    <t>keyword2</t>
+  </si>
+  <si>
+    <t>YLSYtazminat</t>
+  </si>
+  <si>
+    <t>keyword3</t>
+  </si>
+  <si>
+    <t>ylsytazminat</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>abacdsada</t>
+    <t>aaaaaaaa</t>
+  </si>
+  <si>
+    <t>bbbbbbbb</t>
+  </si>
+  <si>
+    <t>ccccccccc</t>
+  </si>
+  <si>
+    <t>dddddddddd</t>
+  </si>
+  <si>
+    <t>eeeeeeee</t>
+  </si>
+  <si>
+    <t>ffff</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +214,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,7 +524,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -523,11 +567,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -561,6 +607,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -881,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -895,9 +942,13 @@
     <col min="4" max="4" width="50.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -911,33 +962,60 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="tanercokyasar@gmail.com" xr:uid="{7E9BC2E7-881D-494D-A031-C024602D87DF}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>